<commit_message>
fix example field value
</commit_message>
<xml_diff>
--- a/data_final/dictionaries/T_Dict.xlsx
+++ b/data_final/dictionaries/T_Dict.xlsx
@@ -358,7 +358,7 @@
     <t xml:space="preserve">Age45_54</t>
   </si>
   <si>
-    <t xml:space="preserve">Total population between 45 and 54 years of age.</t>
+    <t xml:space="preserve">Total population between age 45-54</t>
   </si>
   <si>
     <t xml:space="preserve">IPUMS NHGIS</t>
@@ -1421,8 +1421,8 @@
   </sheetPr>
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O31" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O51" activeCellId="0" sqref="O51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L25" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q37" activeCellId="0" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2875,6 +2875,9 @@
       <c r="O31" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="P31" s="1" t="n">
+        <v>1020</v>
+      </c>
       <c r="R31" s="1" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
add RAAM variables to data dictionary
</commit_message>
<xml_diff>
--- a/data_final/dictionaries/T_Dict.xlsx
+++ b/data_final/dictionaries/T_Dict.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="431">
   <si>
     <t xml:space="preserve">Theme</t>
   </si>
@@ -948,6 +948,132 @@
   </si>
   <si>
     <t xml:space="preserve">Count of naltrexone providers in 30 minute biking time threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetRm30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methadone access 30 minutes (RAAM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetRm60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methadone access 60 minutes (RAAM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetRm90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methadone access 90 minutes (RAAM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NalRm30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naltrexone access 30 minutes (RAAM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NalRm60</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Naltrexone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> access 60 minutes (RAAM)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NalRm90</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Naltrexone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> access 90 minutes (RAAM)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BupRm30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buprenorphine access 30 minutes (RAAM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BupRm60</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Buprenorphine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> access 60 minutes (RAAM)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BupRm90</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Buprenorphine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> access 90 minutes (RAAM)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">FqhcMinDis</t>
@@ -1270,7 +1396,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1300,6 +1426,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1356,7 +1488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1405,6 +1537,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,10 +1558,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ131"/>
+  <dimension ref="A1:AMJ140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q104" activeCellId="0" sqref="Q104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5550,6 +5686,18 @@
       <c r="A100" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="B100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F100" s="2" t="s">
         <v>15</v>
       </c>
@@ -5559,109 +5707,82 @@
       <c r="J100" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="K100" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="L100" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="M100" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="N100" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="O100" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P100" s="1" t="n">
-        <v>10.23</v>
-      </c>
-      <c r="Q100" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R100" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q100" s="6"/>
+      <c r="R100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="B101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F101" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H101" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I101" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="K101" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="L101" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="M101" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="N101" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="O101" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P101" s="1" t="n">
-        <v>19.16</v>
-      </c>
-      <c r="Q101" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R101" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q101" s="6"/>
+      <c r="R101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="B102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F102" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="K102" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="L102" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="M102" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="N102" s="1" t="s">
         <v>314</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="P102" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q102" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R102" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q102" s="6"/>
+      <c r="R102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
@@ -5671,35 +5792,19 @@
         <v>15</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="K103" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="L103" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="M103" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="N103" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="O103" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P103" s="1" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="Q103" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R103" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q103" s="6"/>
+      <c r="R103" s="6"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
@@ -5708,39 +5813,20 @@
       <c r="F104" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H104" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I104" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="K104" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="L104" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="N104" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
+      </c>
+      <c r="J104" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="O104" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P104" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q104" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R104" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q104" s="6"/>
+      <c r="R104" s="6"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
@@ -5750,35 +5836,19 @@
         <v>15</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="K105" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="L105" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="M105" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="N105" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
+      </c>
+      <c r="J105" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="O105" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="P105" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q105" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R105" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="6"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
@@ -5788,35 +5858,19 @@
         <v>15</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="K106" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="L106" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="M106" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="N106" s="1" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="O106" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P106" s="1" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="Q106" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R106" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
@@ -5825,39 +5879,20 @@
       <c r="F107" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H107" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I107" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="J107" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="K107" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="L107" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="M107" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="N107" s="1" t="s">
-        <v>334</v>
+        <v>323</v>
+      </c>
+      <c r="J107" s="12" t="s">
+        <v>324</v>
       </c>
       <c r="O107" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P107" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q107" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R107" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q107" s="6"/>
+      <c r="R107" s="6"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
@@ -5867,35 +5902,19 @@
         <v>15</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="J108" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="L108" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="N108" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
+      </c>
+      <c r="J108" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="O108" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="P108" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="Q108" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="R108" s="6" t="s">
-        <v>316</v>
-      </c>
+        <v>1.232</v>
+      </c>
+      <c r="Q108" s="6"/>
+      <c r="R108" s="6"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
@@ -5905,34 +5924,34 @@
         <v>15</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="O109" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P109" s="1" t="n">
-        <v>0.2</v>
+        <v>10.23</v>
       </c>
       <c r="Q109" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R109" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5946,34 +5965,34 @@
         <v>15</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="O110" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P110" s="1" t="n">
-        <v>0</v>
+        <v>19.16</v>
       </c>
       <c r="Q110" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R110" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,34 +6003,34 @@
         <v>15</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="O111" s="1" t="s">
         <v>48</v>
       </c>
       <c r="P111" s="1" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="Q111" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R111" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6022,34 +6041,34 @@
         <v>15</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="L112" s="1" t="s">
         <v>342</v>
       </c>
       <c r="M112" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N112" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="N112" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="O112" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P112" s="1" t="n">
-        <v>4.99</v>
+        <v>0.31</v>
       </c>
       <c r="Q112" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R112" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6063,34 +6082,34 @@
         <v>15</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="L113" s="1" t="s">
         <v>342</v>
       </c>
       <c r="M113" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N113" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="N113" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="O113" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P113" s="1" t="n">
-        <v>17.76</v>
+        <v>0</v>
       </c>
       <c r="Q113" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R113" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6101,34 +6120,34 @@
         <v>15</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="L114" s="1" t="s">
         <v>342</v>
       </c>
       <c r="M114" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N114" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="N114" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="O114" s="1" t="s">
         <v>48</v>
       </c>
       <c r="P114" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q114" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R114" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6139,34 +6158,34 @@
         <v>15</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="K115" s="8" t="s">
-        <v>359</v>
+        <v>349</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>350</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O115" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P115" s="1" t="n">
-        <v>13.12</v>
+        <v>0.84</v>
       </c>
       <c r="Q115" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R115" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6180,34 +6199,34 @@
         <v>15</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="K116" s="8" t="s">
-        <v>359</v>
+        <v>354</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>350</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="M116" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O116" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P116" s="1" t="n">
-        <v>27.39</v>
+        <v>0</v>
       </c>
       <c r="Q116" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R116" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6218,34 +6237,34 @@
         <v>15</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="K117" s="8" t="s">
-        <v>359</v>
+        <v>356</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>350</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O117" s="1" t="s">
         <v>48</v>
       </c>
       <c r="P117" s="1" t="n">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="Q117" s="6" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="R117" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6255,35 +6274,35 @@
       <c r="F118" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H118" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I118" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="L118" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="M118" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="O118" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="P118" s="1" t="n">
-        <v>13</v>
+        <v>0.2</v>
       </c>
       <c r="Q118" s="6" t="s">
-        <v>373</v>
+        <v>333</v>
+      </c>
+      <c r="R118" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6293,32 +6312,38 @@
       <c r="F119" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H119" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="I119" s="1" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="O119" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="P119" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q119" s="6" t="s">
-        <v>373</v>
+        <v>333</v>
+      </c>
+      <c r="R119" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6328,32 +6353,35 @@
       <c r="F120" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H120" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I120" s="1" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
+      </c>
+      <c r="N120" s="1" t="s">
+        <v>362</v>
       </c>
       <c r="O120" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="P120" s="1" t="n">
-        <v>133.42</v>
+        <v>3</v>
       </c>
       <c r="Q120" s="6" t="s">
-        <v>373</v>
+        <v>333</v>
+      </c>
+      <c r="R120" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6364,33 +6392,39 @@
         <v>15</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="K121" s="1" t="s">
         <v>369</v>
       </c>
       <c r="L121" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="N121" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="M121" s="1" t="s">
-        <v>371</v>
-      </c>
       <c r="O121" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P121" s="1" t="n">
-        <v>41.05</v>
+        <v>4.99</v>
       </c>
       <c r="Q121" s="6" t="s">
-        <v>373</v>
+        <v>333</v>
+      </c>
+      <c r="R121" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>15</v>
@@ -6399,149 +6433,194 @@
         <v>15</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>382</v>
+        <v>372</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>369</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="M122" s="1" t="s">
-        <v>384</v>
+        <v>361</v>
+      </c>
+      <c r="N122" s="1" t="s">
+        <v>370</v>
       </c>
       <c r="O122" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P122" s="1" t="n">
-        <v>1.17</v>
+        <v>17.76</v>
+      </c>
+      <c r="Q122" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="R122" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H123" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I123" s="1" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>386</v>
+        <v>374</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>369</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>384</v>
+        <v>361</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>370</v>
       </c>
       <c r="O123" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="P123" s="1" t="n">
-        <v>0.54</v>
+        <v>4</v>
+      </c>
+      <c r="Q123" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="R123" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K124" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="L124" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="N124" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="F124" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I124" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="J124" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="L124" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="M124" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="O124" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P124" s="1" t="n">
-        <v>-0.06</v>
+        <v>13.12</v>
+      </c>
+      <c r="Q124" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="R124" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K125" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="N125" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="F125" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="J125" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="L125" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="M125" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="O125" s="1" t="s">
         <v>76</v>
       </c>
       <c r="P125" s="1" t="n">
-        <v>0.59</v>
+        <v>27.39</v>
+      </c>
+      <c r="Q125" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="R125" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K126" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="N126" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="F126" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I126" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="J126" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="K126" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="L126" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="M126" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="N126" s="1" t="s">
-        <v>395</v>
-      </c>
       <c r="O126" s="1" t="s">
-        <v>220</v>
+        <v>48</v>
       </c>
       <c r="P126" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q126" s="1" t="s">
-        <v>396</v>
+        <v>1</v>
+      </c>
+      <c r="Q126" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="R126" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>15</v>
@@ -6550,174 +6629,465 @@
         <v>15</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="M127" s="1" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="O127" s="1" t="s">
-        <v>403</v>
+        <v>48</v>
       </c>
       <c r="P127" s="1" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="Q127" s="1" t="s">
-        <v>404</v>
+        <v>13</v>
+      </c>
+      <c r="Q127" s="6" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="L128" s="1" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="O128" s="1" t="s">
-        <v>403</v>
+        <v>48</v>
       </c>
       <c r="P128" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Q128" s="1" t="s">
-        <v>404</v>
+        <v>4</v>
+      </c>
+      <c r="Q128" s="6" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H129" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="I129" s="1" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="N129" s="1" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="O129" s="1" t="s">
-        <v>403</v>
+        <v>76</v>
       </c>
       <c r="P129" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Q129" s="1" t="s">
-        <v>404</v>
+        <v>133.42</v>
+      </c>
+      <c r="Q129" s="6" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H130" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I130" s="1" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="N130" s="1" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="O130" s="1" t="s">
-        <v>403</v>
+        <v>76</v>
       </c>
       <c r="P130" s="1" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="Q130" s="1" t="s">
-        <v>404</v>
+        <v>41.05</v>
+      </c>
+      <c r="Q130" s="6" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H131" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="I131" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="L131" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="O131" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P131" s="1" t="n">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="L132" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P132" s="1" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="J133" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="L133" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P133" s="1" t="n">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="L134" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P134" s="1" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="K135" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="J131" s="1" t="s">
+      <c r="L135" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="K131" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="L131" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="M131" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="N131" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="O131" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="P131" s="1" t="n">
+      <c r="M135" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="N135" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="P135" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q135" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="N136" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="P136" s="1" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="Q136" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="P137" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Q137" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="N138" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="P138" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q138" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="P139" s="1" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="Q139" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="P140" s="1" t="n">
         <v>0.38</v>
       </c>
-      <c r="Q131" s="1" t="s">
-        <v>404</v>
+      <c r="Q140" s="1" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>